<commit_message>
cleanUP escena_04 frm 21-41
</commit_message>
<xml_diff>
--- a/Tiempos_Escenas.xlsx
+++ b/Tiempos_Escenas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pablo\Andrea\USFQ\Titulacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBB198E-24BB-4238-A6FE-46E8B7131704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905B96A1-4E9F-41AB-A71C-ADC4F6E8BD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7479791D-AF98-4B48-9BA8-5A6EBE4D9B1A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="107">
   <si>
     <t>Escenas</t>
   </si>
@@ -353,6 +353,12 @@
   </si>
   <si>
     <t>Begin Date:</t>
+  </si>
+  <si>
+    <t>CleanUp</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -515,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -562,11 +568,67 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -584,40 +646,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -683,6 +712,48 @@
         </patternFill>
       </fill>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -870,6 +941,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -879,13 +957,6 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -929,6 +1000,119 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -954,9 +1138,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Escenas_style" pivot="0" count="3" xr9:uid="{2A99205D-6212-4C05-8828-38A2C5030BE6}">
-      <tableStyleElement type="headerRow" dxfId="14"/>
-      <tableStyleElement type="totalRow" dxfId="13"/>
-      <tableStyleElement type="secondRowStripe" dxfId="12"/>
+      <tableStyleElement type="headerRow" dxfId="30"/>
+      <tableStyleElement type="totalRow" dxfId="29"/>
+      <tableStyleElement type="secondRowStripe" dxfId="28"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -971,18 +1155,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8D524042-5AAD-4EFE-A25F-7BF55D11B420}" name="Table2" displayName="Table2" ref="A1:G82" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="A1:G82" xr:uid="{8D524042-5AAD-4EFE-A25F-7BF55D11B420}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{EEB0F2DB-5A60-45E2-B42A-7F3A777A60FD}" name="Column1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{366908A8-A1EE-4A6A-84F5-5A7E1B687F76}" name="Escenas" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{F1850ADF-8A29-4D65-A2DF-6BCB825069D9}" name="Frames" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{8D6B2F7F-5281-49B3-9FFD-4F7E12628708}" name="Seg" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{445C2CF8-A5A5-4A8A-B64A-B0A91BA13D34}" name="Tiempo" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8D524042-5AAD-4EFE-A25F-7BF55D11B420}" name="Table2" displayName="Table2" ref="A1:H82" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+  <autoFilter ref="A1:H82" xr:uid="{8D524042-5AAD-4EFE-A25F-7BF55D11B420}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{EEB0F2DB-5A60-45E2-B42A-7F3A777A60FD}" name="Column1" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{366908A8-A1EE-4A6A-84F5-5A7E1B687F76}" name="Escenas" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{F1850ADF-8A29-4D65-A2DF-6BCB825069D9}" name="Frames" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{8D6B2F7F-5281-49B3-9FFD-4F7E12628708}" name="Seg" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{445C2CF8-A5A5-4A8A-B64A-B0A91BA13D34}" name="Tiempo" dataDxfId="8">
       <calculatedColumnFormula>IF(D2=0,"",_xlfn.CONCAT(TEXT(INT(D2/60),"00"),":",TEXT(MOD(D2,60),"00.00")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{53E24129-A6A4-4D4A-9FB0-A2036B18656E}" name="SegTr" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{89D4FAB2-8B5E-4C99-A020-3A3C601CAF35}" name="Transcurrido" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{53E24129-A6A4-4D4A-9FB0-A2036B18656E}" name="SegTr" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{89D4FAB2-8B5E-4C99-A020-3A3C601CAF35}" name="Transcurrido" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{521AEA72-C192-4798-A8AA-4A0EA4F73489}" name="CleanUp" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="Escenas_style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1312,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C6AA15-B2AD-42A1-BDDC-F5ADA737CF93}">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1326,10 +1511,11 @@
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="8.21875" customWidth="1"/>
     <col min="7" max="7" width="13.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
@@ -1351,8 +1537,11 @@
       <c r="G1" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1376,8 +1565,10 @@
         <f>_xlfn.CONCAT(TEXT(INT(F2/60),"00"),":",TEXT(MOD(F2,60),"00.00"))</f>
         <v>00:00.00</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1403,8 +1594,9 @@
         <f>IF(D3=0,"",_xlfn.CONCAT(TEXT(INT(F3/60),"00"),":",TEXT(MOD(F3,60),"00.00")))</f>
         <v>00:04.54</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1430,33 +1622,37 @@
         <f t="shared" ref="G4:G67" si="3">IF(D4=0,"",_xlfn.CONCAT(TEXT(INT(F4/60),"00"),":",TEXT(MOD(F4,60),"00.00")))</f>
         <v>00:07.46</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4">
+        <v>41</v>
+      </c>
       <c r="D5" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.7083333333333333</v>
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>00:01.71</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="2"/>
-        <v>7.4583333333333339</v>
+        <v>9.1666666666666679</v>
       </c>
       <c r="G5" s="7" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>00:09.17</v>
+      </c>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1476,14 +1672,15 @@
       </c>
       <c r="F6" s="5">
         <f t="shared" si="2"/>
-        <v>10.125</v>
+        <v>11.833333333333334</v>
       </c>
       <c r="G6" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>00:10.13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>00:11.83</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1501,14 +1698,15 @@
       </c>
       <c r="F7" s="5">
         <f t="shared" si="2"/>
-        <v>10.125</v>
+        <v>11.833333333333334</v>
       </c>
       <c r="G7" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1528,14 +1726,15 @@
       </c>
       <c r="F8" s="5">
         <f t="shared" si="2"/>
-        <v>23.458333333333336</v>
+        <v>25.166666666666668</v>
       </c>
       <c r="G8" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>00:23.46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>00:25.17</v>
+      </c>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1555,14 +1754,15 @@
       </c>
       <c r="F9" s="5">
         <f t="shared" si="2"/>
-        <v>26.708333333333336</v>
+        <v>28.416666666666668</v>
       </c>
       <c r="G9" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>00:26.71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>00:28.42</v>
+      </c>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1580,14 +1780,15 @@
       </c>
       <c r="F10" s="5">
         <f t="shared" si="2"/>
-        <v>26.708333333333336</v>
+        <v>28.416666666666668</v>
       </c>
       <c r="G10" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1605,14 +1806,15 @@
       </c>
       <c r="F11" s="5">
         <f t="shared" si="2"/>
-        <v>26.708333333333336</v>
+        <v>28.416666666666668</v>
       </c>
       <c r="G11" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1632,14 +1834,15 @@
       </c>
       <c r="F12" s="5">
         <f t="shared" si="2"/>
-        <v>29.375000000000004</v>
+        <v>31.083333333333336</v>
       </c>
       <c r="G12" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>00:29.38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>00:31.08</v>
+      </c>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -1657,14 +1860,15 @@
       </c>
       <c r="F13" s="5">
         <f t="shared" si="2"/>
-        <v>29.375000000000004</v>
+        <v>31.083333333333336</v>
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -1684,14 +1888,15 @@
       </c>
       <c r="F14" s="5">
         <f t="shared" si="2"/>
-        <v>32.708333333333336</v>
+        <v>34.416666666666671</v>
       </c>
       <c r="G14" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>00:32.71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>00:34.42</v>
+      </c>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -1711,14 +1916,15 @@
       </c>
       <c r="F15" s="5">
         <f t="shared" si="2"/>
-        <v>37.791666666666671</v>
+        <v>39.500000000000007</v>
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>00:37.79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>00:39.50</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -1738,14 +1944,15 @@
       </c>
       <c r="F16" s="5">
         <f t="shared" si="2"/>
-        <v>40.958333333333336</v>
+        <v>42.666666666666671</v>
       </c>
       <c r="G16" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>00:40.96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>00:42.67</v>
+      </c>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -1763,14 +1970,15 @@
       </c>
       <c r="F17" s="5">
         <f t="shared" si="2"/>
-        <v>40.958333333333336</v>
+        <v>42.666666666666671</v>
       </c>
       <c r="G17" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -1790,14 +1998,15 @@
       </c>
       <c r="F18" s="5">
         <f t="shared" si="2"/>
-        <v>42.75</v>
+        <v>44.458333333333336</v>
       </c>
       <c r="G18" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>00:42.75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>00:44.46</v>
+      </c>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -1817,14 +2026,15 @@
       </c>
       <c r="F19" s="5">
         <f t="shared" si="2"/>
-        <v>48.333333333333336</v>
+        <v>50.041666666666671</v>
       </c>
       <c r="G19" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>00:48.33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>00:50.04</v>
+      </c>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -1844,14 +2054,15 @@
       </c>
       <c r="F20" s="5">
         <f t="shared" si="2"/>
-        <v>54.791666666666671</v>
+        <v>56.500000000000007</v>
       </c>
       <c r="G20" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>00:54.79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>00:56.50</v>
+      </c>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -1871,14 +2082,15 @@
       </c>
       <c r="F21" s="5">
         <f t="shared" si="2"/>
-        <v>59.666666666666671</v>
+        <v>61.375000000000007</v>
       </c>
       <c r="G21" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>00:59.67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>01:01.38</v>
+      </c>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -1898,14 +2110,15 @@
       </c>
       <c r="F22" s="5">
         <f t="shared" si="2"/>
-        <v>62.000000000000007</v>
+        <v>63.708333333333343</v>
       </c>
       <c r="G22" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>01:02.00</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>01:03.71</v>
+      </c>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -1923,14 +2136,15 @@
       </c>
       <c r="F23" s="5">
         <f t="shared" si="2"/>
-        <v>62.000000000000007</v>
+        <v>63.708333333333343</v>
       </c>
       <c r="G23" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -1950,14 +2164,15 @@
       </c>
       <c r="F24" s="5">
         <f t="shared" si="2"/>
-        <v>65.625</v>
+        <v>67.333333333333343</v>
       </c>
       <c r="G24" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>01:05.63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>01:07.33</v>
+      </c>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -1977,14 +2192,15 @@
       </c>
       <c r="F25" s="5">
         <f t="shared" si="2"/>
-        <v>66.916666666666671</v>
+        <v>68.625000000000014</v>
       </c>
       <c r="G25" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>01:06.92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>01:08.63</v>
+      </c>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -2004,14 +2220,15 @@
       </c>
       <c r="F26" s="5">
         <f t="shared" si="2"/>
-        <v>71.5</v>
+        <v>73.208333333333343</v>
       </c>
       <c r="G26" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>01:11.50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>01:13.21</v>
+      </c>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -2031,14 +2248,15 @@
       </c>
       <c r="F27" s="5">
         <f t="shared" si="2"/>
-        <v>78.416666666666671</v>
+        <v>80.125000000000014</v>
       </c>
       <c r="G27" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>01:18.42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>01:20.13</v>
+      </c>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -2058,14 +2276,15 @@
       </c>
       <c r="F28" s="5">
         <f t="shared" si="2"/>
-        <v>81.375</v>
+        <v>83.083333333333343</v>
       </c>
       <c r="G28" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>01:21.38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>01:23.08</v>
+      </c>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -2085,14 +2304,15 @@
       </c>
       <c r="F29" s="5">
         <f t="shared" si="2"/>
-        <v>83.5</v>
+        <v>85.208333333333343</v>
       </c>
       <c r="G29" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>01:23.50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>01:25.21</v>
+      </c>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -2110,14 +2330,15 @@
       </c>
       <c r="F30" s="5">
         <f t="shared" si="2"/>
-        <v>83.5</v>
+        <v>85.208333333333343</v>
       </c>
       <c r="G30" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -2137,14 +2358,17 @@
       </c>
       <c r="F31" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G31" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>01:24.88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>01:26.58</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -2162,14 +2386,15 @@
       </c>
       <c r="F32" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G32" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -2187,14 +2412,15 @@
       </c>
       <c r="F33" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G33" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -2212,14 +2438,15 @@
       </c>
       <c r="F34" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G34" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -2237,14 +2464,15 @@
       </c>
       <c r="F35" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G35" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -2262,14 +2490,15 @@
       </c>
       <c r="F36" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G36" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36" s="7"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -2287,14 +2516,15 @@
       </c>
       <c r="F37" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G37" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37" s="7"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>37</v>
       </c>
@@ -2312,14 +2542,15 @@
       </c>
       <c r="F38" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G38" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38" s="7"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>38</v>
       </c>
@@ -2337,14 +2568,15 @@
       </c>
       <c r="F39" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G39" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39" s="7"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>39</v>
       </c>
@@ -2362,14 +2594,15 @@
       </c>
       <c r="F40" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G40" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40" s="7"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>40</v>
       </c>
@@ -2387,14 +2620,15 @@
       </c>
       <c r="F41" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G41" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H41" s="7"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>41</v>
       </c>
@@ -2412,14 +2646,15 @@
       </c>
       <c r="F42" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G42" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42" s="7"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>42</v>
       </c>
@@ -2437,14 +2672,15 @@
       </c>
       <c r="F43" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G43" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H43" s="7"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>43</v>
       </c>
@@ -2462,14 +2698,15 @@
       </c>
       <c r="F44" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G44" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>44</v>
       </c>
@@ -2487,14 +2724,15 @@
       </c>
       <c r="F45" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G45" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H45" s="7"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>45</v>
       </c>
@@ -2512,14 +2750,15 @@
       </c>
       <c r="F46" s="5">
         <f t="shared" si="2"/>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="G46" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H46" s="7"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>46</v>
       </c>
@@ -2539,14 +2778,15 @@
       </c>
       <c r="F47" s="5">
         <f t="shared" si="2"/>
-        <v>89.708333333333329</v>
+        <v>91.416666666666671</v>
       </c>
       <c r="G47" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>01:29.71</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+        <v>01:31.42</v>
+      </c>
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>47</v>
       </c>
@@ -2566,14 +2806,15 @@
       </c>
       <c r="F48" s="5">
         <f t="shared" si="2"/>
-        <v>91.333333333333329</v>
+        <v>93.041666666666671</v>
       </c>
       <c r="G48" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>01:31.33</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+        <v>01:33.04</v>
+      </c>
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>48</v>
       </c>
@@ -2593,14 +2834,15 @@
       </c>
       <c r="F49" s="5">
         <f t="shared" si="2"/>
-        <v>95.291666666666657</v>
+        <v>97</v>
       </c>
       <c r="G49" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>01:35.29</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+        <v>01:37.00</v>
+      </c>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>49</v>
       </c>
@@ -2618,14 +2860,15 @@
       </c>
       <c r="F50" s="5">
         <f t="shared" si="2"/>
-        <v>95.291666666666657</v>
+        <v>97</v>
       </c>
       <c r="G50" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>50</v>
       </c>
@@ -2643,14 +2886,15 @@
       </c>
       <c r="F51" s="5">
         <f t="shared" si="2"/>
-        <v>95.291666666666657</v>
+        <v>97</v>
       </c>
       <c r="G51" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H51" s="7"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>51</v>
       </c>
@@ -2668,14 +2912,15 @@
       </c>
       <c r="F52" s="5">
         <f t="shared" si="2"/>
-        <v>95.291666666666657</v>
+        <v>97</v>
       </c>
       <c r="G52" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>52</v>
       </c>
@@ -2693,14 +2938,15 @@
       </c>
       <c r="F53" s="5">
         <f t="shared" si="2"/>
-        <v>95.291666666666657</v>
+        <v>97</v>
       </c>
       <c r="G53" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H53" s="7"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>53</v>
       </c>
@@ -2720,14 +2966,15 @@
       </c>
       <c r="F54" s="5">
         <f t="shared" si="2"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G54" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>01:36.71</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+        <v>01:38.42</v>
+      </c>
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>54</v>
       </c>
@@ -2745,14 +2992,15 @@
       </c>
       <c r="F55" s="5">
         <f t="shared" si="2"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G55" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>55</v>
       </c>
@@ -2770,14 +3018,15 @@
       </c>
       <c r="F56" s="5">
         <f t="shared" si="2"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G56" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <v>56</v>
       </c>
@@ -2795,14 +3044,15 @@
       </c>
       <c r="F57" s="5">
         <f t="shared" si="2"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G57" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H57" s="7"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <v>57</v>
       </c>
@@ -2820,14 +3070,15 @@
       </c>
       <c r="F58" s="5">
         <f t="shared" si="2"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G58" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H58" s="7"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <v>58</v>
       </c>
@@ -2845,14 +3096,15 @@
       </c>
       <c r="F59" s="5">
         <f t="shared" si="2"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G59" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>59</v>
       </c>
@@ -2870,14 +3122,15 @@
       </c>
       <c r="F60" s="5">
         <f t="shared" si="2"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G60" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>60</v>
       </c>
@@ -2895,14 +3148,15 @@
       </c>
       <c r="F61" s="5">
         <f t="shared" si="2"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G61" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <v>61</v>
       </c>
@@ -2920,14 +3174,15 @@
       </c>
       <c r="F62" s="5">
         <f t="shared" si="2"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G62" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -2945,14 +3200,15 @@
       </c>
       <c r="F63" s="5">
         <f t="shared" si="2"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G63" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H63" s="7"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <v>63</v>
       </c>
@@ -2970,14 +3226,15 @@
       </c>
       <c r="F64" s="5">
         <f t="shared" si="2"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G64" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
         <v>64</v>
       </c>
@@ -2995,14 +3252,15 @@
       </c>
       <c r="F65" s="5">
         <f t="shared" si="2"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G65" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H65" s="7"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <v>65</v>
       </c>
@@ -3015,19 +3273,20 @@
         <v>0</v>
       </c>
       <c r="E66" s="3" t="str">
-        <f t="shared" ref="E66:E97" si="6">IF(D66=0,"",_xlfn.CONCAT(TEXT(INT(D66/60),"00"),":",TEXT(MOD(D66,60),"00.00")))</f>
+        <f t="shared" ref="E66:E82" si="6">IF(D66=0,"",_xlfn.CONCAT(TEXT(INT(D66/60),"00"),":",TEXT(MOD(D66,60),"00.00")))</f>
         <v/>
       </c>
       <c r="F66" s="5">
         <f t="shared" si="2"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G66" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H66" s="7"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <v>66</v>
       </c>
@@ -3045,14 +3304,15 @@
       </c>
       <c r="F67" s="5">
         <f t="shared" si="2"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G67" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H67" s="7"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>67</v>
       </c>
@@ -3070,14 +3330,15 @@
       </c>
       <c r="F68" s="5">
         <f t="shared" ref="F68:F81" si="7">F67+D68</f>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G68" s="7" t="str">
         <f t="shared" ref="G68:G81" si="8">IF(D68=0,"",_xlfn.CONCAT(TEXT(INT(F68/60),"00"),":",TEXT(MOD(F68,60),"00.00")))</f>
         <v/>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H68" s="7"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>68</v>
       </c>
@@ -3095,14 +3356,15 @@
       </c>
       <c r="F69" s="5">
         <f t="shared" si="7"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G69" s="7" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H69" s="7"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -3120,14 +3382,15 @@
       </c>
       <c r="F70" s="5">
         <f t="shared" si="7"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G70" s="7" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H70" s="7"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
         <v>70</v>
       </c>
@@ -3145,14 +3408,15 @@
       </c>
       <c r="F71" s="5">
         <f t="shared" si="7"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G71" s="7" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H71" s="7"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -3170,14 +3434,15 @@
       </c>
       <c r="F72" s="5">
         <f t="shared" si="7"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G72" s="7" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H72" s="7"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
         <v>72</v>
       </c>
@@ -3195,14 +3460,15 @@
       </c>
       <c r="F73" s="5">
         <f t="shared" si="7"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G73" s="7" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H73" s="7"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <v>73</v>
       </c>
@@ -3220,14 +3486,15 @@
       </c>
       <c r="F74" s="5">
         <f t="shared" si="7"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G74" s="7" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H74" s="7"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
         <v>74</v>
       </c>
@@ -3245,14 +3512,15 @@
       </c>
       <c r="F75" s="5">
         <f t="shared" si="7"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G75" s="7" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H75" s="7"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="6">
         <v>75</v>
       </c>
@@ -3270,14 +3538,15 @@
       </c>
       <c r="F76" s="5">
         <f t="shared" si="7"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G76" s="7" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H76" s="7"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="6">
         <v>76</v>
       </c>
@@ -3295,14 +3564,15 @@
       </c>
       <c r="F77" s="5">
         <f t="shared" si="7"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G77" s="7" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H77" s="7"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="6">
         <v>77</v>
       </c>
@@ -3320,14 +3590,15 @@
       </c>
       <c r="F78" s="5">
         <f t="shared" si="7"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G78" s="7" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H78" s="7"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="6">
         <v>78</v>
       </c>
@@ -3345,14 +3616,15 @@
       </c>
       <c r="F79" s="5">
         <f t="shared" si="7"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G79" s="7" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H79" s="7"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="6">
         <v>79</v>
       </c>
@@ -3370,14 +3642,15 @@
       </c>
       <c r="F80" s="5">
         <f t="shared" si="7"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G80" s="7" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H80" s="7"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="6">
         <v>80</v>
       </c>
@@ -3395,14 +3668,15 @@
       </c>
       <c r="F81" s="5">
         <f t="shared" si="7"/>
-        <v>96.708333333333329</v>
+        <v>98.416666666666671</v>
       </c>
       <c r="G81" s="7" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H81" s="7"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="11">
         <f>COUNT(A2:A81)</f>
         <v>80</v>
@@ -3412,31 +3686,43 @@
       </c>
       <c r="C82" s="13">
         <f>SUM(C2:C42)</f>
-        <v>2037</v>
+        <v>2078</v>
       </c>
       <c r="D82" s="14">
         <f>SUM(D2:D42)</f>
-        <v>84.875</v>
+        <v>86.583333333333343</v>
       </c>
       <c r="E82" s="15" t="str">
         <f t="shared" si="6"/>
-        <v>01:24.88</v>
+        <v>01:26.58</v>
       </c>
       <c r="F82" s="13"/>
       <c r="G82" s="16"/>
+      <c r="H82" s="18"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C81">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="2">
+      <formula>LEN(TRIM(I2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H81">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(H2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="F2:F4 F5:F81" formula="1"/>
   </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>